<commit_message>
Adding GEDCOM and organising files
</commit_message>
<xml_diff>
--- a/Excel Sheet/Team_DhruvalKunjNihirVyomYash_Report.xlsx
+++ b/Excel Sheet/Team_DhruvalKunjNihirVyomYash_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhruval\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunj/Desktop/Stevens/CS555_Final_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA42927-0E12-4198-BC16-0E342A8E2920}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30D1501-0C03-9B49-8776-ACC43043266B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15720" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="230">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -118,10 +118,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Story Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -150,18 +146,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Story ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Owner</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Sprint</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -538,175 +522,244 @@
     <t>US42</t>
   </si>
   <si>
+    <t>Dates before current date</t>
+  </si>
+  <si>
+    <t>Birth before marriage of parents</t>
+  </si>
+  <si>
+    <t>The goal of the burndown chart is to help the agile team and customer to understand how the developers are doing</t>
+  </si>
+  <si>
+    <t>to deliver the product.  Burndown charts can be done daily, weekly, at the end of a sprint, or at whatever time interval makes sense.</t>
+  </si>
+  <si>
+    <t>We'll update our burndown chart for the GEDCOM project at the end of each sprint.</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>At the end of each sprint, you should update the number of remaining stories, the LOC written to implement the user stories</t>
+  </si>
+  <si>
+    <t>implemented in this sprint, and the minutes needed to write those lines of code.</t>
+  </si>
+  <si>
+    <t>Here's a sample burndown chart for a team of three:</t>
+  </si>
+  <si>
+    <t>Multiple births &lt;= 5</t>
+  </si>
+  <si>
+    <t>Children should be born after marriage of parents (and not more than 9 months after their divorce)</t>
+  </si>
+  <si>
+    <t>Marriage should be at least 14 years after birth of both spouses (parents must be at least 14 years old)</t>
+  </si>
+  <si>
+    <t>Birth dates of siblings should be more than 8 months apart or less than 2 days apart (twins may be born one day apart, e.g. 11:59 PM and 12:02 AM the following calendar day)</t>
+  </si>
+  <si>
+    <t>All family roles (spouse, child) specified in an individual record should have corresponding entries in the corresponding family records. Likewise, all individual roles (spouse, child) specified in family records should have corresponding entries in the corresponding  individual's records.  I.e. the information in the individual and family records should be consistent.</t>
+  </si>
+  <si>
+    <t>List siblings in families by decreasing age, i.e. oldest siblings first</t>
+  </si>
+  <si>
+    <t>Parents should not marry any of their children</t>
+  </si>
+  <si>
+    <t>No marriages to children</t>
+  </si>
+  <si>
+    <t>Source File</t>
+  </si>
+  <si>
+    <t>Test File</t>
+  </si>
+  <si>
+    <t>Source Function</t>
+  </si>
+  <si>
+    <t>Source Lines</t>
+  </si>
+  <si>
+    <t>Test Function</t>
+  </si>
+  <si>
+    <t>Test lines</t>
+  </si>
+  <si>
+    <t>KD</t>
+  </si>
+  <si>
+    <t>Kunj</t>
+  </si>
+  <si>
+    <t>Desai</t>
+  </si>
+  <si>
+    <t>Nihir</t>
+  </si>
+  <si>
+    <t>Patel</t>
+  </si>
+  <si>
+    <t>NP</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>Dhruval</t>
+  </si>
+  <si>
+    <t>Thakkar</t>
+  </si>
+  <si>
+    <t>dthakka3@stevens.edu</t>
+  </si>
+  <si>
+    <t>Dhruval16</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>Vyom</t>
+  </si>
+  <si>
+    <t>Shah</t>
+  </si>
+  <si>
+    <t>YN</t>
+  </si>
+  <si>
+    <t>Yash</t>
+  </si>
+  <si>
+    <t>Navadiya</t>
+  </si>
+  <si>
+    <t>https://github.com/KunjDesai96/CS555_Final_Project</t>
+  </si>
+  <si>
+    <t>KunjDesai96</t>
+  </si>
+  <si>
+    <t>kdedai11@stevens.edu</t>
+  </si>
+  <si>
+    <t>npate76@stevens.edu</t>
+  </si>
+  <si>
+    <t>Nihir108</t>
+  </si>
+  <si>
+    <t>vshah50@stevens.edu</t>
+  </si>
+  <si>
+    <t>Vyom0123</t>
+  </si>
+  <si>
+    <t>Yashnavadiya</t>
+  </si>
+  <si>
+    <t>ynavadiy@stevens.edu</t>
+  </si>
+  <si>
+    <t>Unique Ids</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>GenerateOutput</t>
+  </si>
+  <si>
+    <t>us02_birth_b4_marriage</t>
+  </si>
+  <si>
+    <t>us04_marriage_b4_divorce</t>
+  </si>
+  <si>
+    <t>GenerateOutputTest</t>
+  </si>
+  <si>
+    <t>test_us02_birth_b4_marriage</t>
+  </si>
+  <si>
+    <t>test_us04_marriage_b4_divorce</t>
+  </si>
+  <si>
+    <t>29-35</t>
+  </si>
+  <si>
+    <t>20-26</t>
+  </si>
+  <si>
+    <t>List Upcoming birthdays</t>
+  </si>
+  <si>
+    <t>us06_divorce_b4_death()</t>
+  </si>
+  <si>
+    <t>test_us06_divorce_b4_death()</t>
+  </si>
+  <si>
     <t>Coding</t>
   </si>
   <si>
-    <t>Dates before current date</t>
-  </si>
-  <si>
-    <t>Birth before marriage of parents</t>
-  </si>
-  <si>
-    <t>The goal of the burndown chart is to help the agile team and customer to understand how the developers are doing</t>
-  </si>
-  <si>
-    <t>to deliver the product.  Burndown charts can be done daily, weekly, at the end of a sprint, or at whatever time interval makes sense.</t>
-  </si>
-  <si>
-    <t>We'll update our burndown chart for the GEDCOM project at the end of each sprint.</t>
-  </si>
-  <si>
-    <t>Sprint</t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>Sprint 2</t>
-  </si>
-  <si>
-    <t>Sprint 3</t>
-  </si>
-  <si>
-    <t>Sprint 4</t>
-  </si>
-  <si>
-    <t>At the end of each sprint, you should update the number of remaining stories, the LOC written to implement the user stories</t>
-  </si>
-  <si>
-    <t>implemented in this sprint, and the minutes needed to write those lines of code.</t>
-  </si>
-  <si>
-    <t>Here's a sample burndown chart for a team of three:</t>
-  </si>
-  <si>
-    <t>Multiple births &lt;= 5</t>
-  </si>
-  <si>
-    <t>Children should be born after marriage of parents (and not more than 9 months after their divorce)</t>
-  </si>
-  <si>
-    <t>Marriage should be at least 14 years after birth of both spouses (parents must be at least 14 years old)</t>
-  </si>
-  <si>
-    <t>Birth dates of siblings should be more than 8 months apart or less than 2 days apart (twins may be born one day apart, e.g. 11:59 PM and 12:02 AM the following calendar day)</t>
-  </si>
-  <si>
-    <t>All family roles (spouse, child) specified in an individual record should have corresponding entries in the corresponding family records. Likewise, all individual roles (spouse, child) specified in family records should have corresponding entries in the corresponding  individual's records.  I.e. the information in the individual and family records should be consistent.</t>
-  </si>
-  <si>
-    <t>List siblings in families by decreasing age, i.e. oldest siblings first</t>
-  </si>
-  <si>
-    <t>Parents should not marry any of their children</t>
-  </si>
-  <si>
-    <t>No marriages to children</t>
-  </si>
-  <si>
-    <t>Source File</t>
-  </si>
-  <si>
-    <t>Test File</t>
-  </si>
-  <si>
-    <t>Source Function</t>
-  </si>
-  <si>
-    <t>Source Lines</t>
-  </si>
-  <si>
-    <t>Test Function</t>
-  </si>
-  <si>
-    <t>Test lines</t>
-  </si>
-  <si>
-    <t>KD</t>
-  </si>
-  <si>
-    <t>Kunj</t>
-  </si>
-  <si>
-    <t>Desai</t>
-  </si>
-  <si>
-    <t>Nihir</t>
-  </si>
-  <si>
-    <t>Patel</t>
-  </si>
-  <si>
-    <t>NP</t>
-  </si>
-  <si>
-    <t>DT</t>
-  </si>
-  <si>
-    <t>Dhruval</t>
-  </si>
-  <si>
-    <t>Thakkar</t>
-  </si>
-  <si>
-    <t>dthakka3@stevens.edu</t>
-  </si>
-  <si>
-    <t>Dhruval16</t>
-  </si>
-  <si>
-    <t>VS</t>
-  </si>
-  <si>
-    <t>Vyom</t>
-  </si>
-  <si>
-    <t>Shah</t>
-  </si>
-  <si>
-    <t>YN</t>
-  </si>
-  <si>
-    <t>Yash</t>
-  </si>
-  <si>
-    <t>Navadiya</t>
-  </si>
-  <si>
-    <t>https://github.com/KunjDesai96/CS555_Final_Project</t>
-  </si>
-  <si>
-    <t>KunjDesai96</t>
-  </si>
-  <si>
-    <t>kdedai11@stevens.edu</t>
-  </si>
-  <si>
-    <t>npate76@stevens.edu</t>
-  </si>
-  <si>
-    <t>Nihir108</t>
-  </si>
-  <si>
-    <t>vshah50@stevens.edu</t>
-  </si>
-  <si>
-    <t>Vyom0123</t>
-  </si>
-  <si>
-    <t>Yashnavadiya</t>
-  </si>
-  <si>
-    <t>ynavadiy@stevens.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding </t>
-  </si>
-  <si>
-    <t>Unique Ids</t>
+    <t>1.5 hours</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>Spending time on writing code and reusing the code</t>
+  </si>
+  <si>
+    <t>48-54</t>
+  </si>
+  <si>
+    <t>174-220</t>
+  </si>
+  <si>
+    <t>us10_marriage_after_14()</t>
+  </si>
+  <si>
+    <t>231-277</t>
+  </si>
+  <si>
+    <t>test_us10_marriage_after_14()</t>
+  </si>
+  <si>
+    <t>57-63</t>
+  </si>
+  <si>
+    <t>33-79</t>
+  </si>
+  <si>
+    <t>89-122</t>
   </si>
 </sst>
 </file>
@@ -717,7 +770,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -762,6 +815,12 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -855,7 +914,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -892,6 +951,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="65"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1001,10 +1069,16 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42409</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42430</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42451</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1017,6 +1091,12 @@
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1048,7 +1128,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1119,6 +1199,9 @@
                 <c:pt idx="0">
                   <c:v>42409</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>42430</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1130,6 +1213,9 @@
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2023,123 +2109,123 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.453125" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
-    <col min="5" max="5" width="45.26953125" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>183</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="E4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>184</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B5" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="C5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="E5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="E7" t="s">
         <v>202</v>
       </c>
-      <c r="E3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" t="s">
-        <v>187</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="E4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>189</v>
-      </c>
-      <c r="B5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C5" t="s">
-        <v>191</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="E5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
         <v>195</v>
-      </c>
-      <c r="C6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="E6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>197</v>
-      </c>
-      <c r="B7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="E7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2161,210 +2247,632 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D11"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>188</v>
-      </c>
-      <c r="E6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>188</v>
-      </c>
-      <c r="E7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
         <v>119</v>
       </c>
-      <c r="C11" t="s">
-        <v>156</v>
-      </c>
-      <c r="D11" t="s">
-        <v>197</v>
-      </c>
-      <c r="E11" t="s">
-        <v>154</v>
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E41">
+    <sortCondition ref="A1"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{C83A676B-2FD1-CB48-8DB4-7BBF8C157176}">
+      <formula1>"Pending, Coding, Completed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -2374,53 +2882,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="67" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -2432,18 +2940,18 @@
         <v>2</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B15" s="13">
         <v>42409</v>
@@ -2455,12 +2963,16 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>162</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
+        <v>157</v>
+      </c>
+      <c r="B16" s="13">
+        <v>42430</v>
+      </c>
+      <c r="C16" s="14">
+        <v>30</v>
+      </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="9" t="e">
@@ -2468,12 +2980,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
+        <v>158</v>
+      </c>
+      <c r="B17" s="13">
+        <v>42451</v>
+      </c>
+      <c r="C17" s="14">
+        <v>20</v>
+      </c>
       <c r="E17" s="14"/>
       <c r="F17" s="15"/>
       <c r="G17" s="9" t="e">
@@ -2481,9 +2997,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="14"/>
@@ -2494,9 +3010,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="14"/>
@@ -2519,20 +3035,20 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2543,16 +3059,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>42409</v>
       </c>
@@ -2563,7 +3079,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="2">
+        <v>42430</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
       <c r="F3" s="9" t="e">
         <f>(D3-D2)/E3*60</f>
         <v>#DIV/0!</v>
@@ -2581,31 +3103,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="105" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="27.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.453125" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.83203125" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.81640625" style="17" customWidth="1"/>
-    <col min="15" max="15" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.453125" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2634,42 +3156,72 @@
         <v>17</v>
       </c>
       <c r="K1" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q1" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="L1" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="O1" s="16" t="s">
+    </row>
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="P1" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2">
+        <v>60</v>
+      </c>
+      <c r="F2" s="21">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <v>46</v>
+      </c>
+      <c r="H2">
+        <v>45</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="4"/>
@@ -2681,100 +3233,136 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+      <c r="D4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4">
+        <v>70</v>
+      </c>
+      <c r="F4">
+        <v>120</v>
+      </c>
+      <c r="G4">
+        <v>33</v>
+      </c>
+      <c r="H4" s="21">
+        <v>90</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="P4" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="4"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="L14" s="18"/>
       <c r="M14" s="18"/>
@@ -2782,7 +3370,7 @@
       <c r="P14" s="18"/>
       <c r="Q14" s="18"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2793,71 +3381,85 @@
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B25" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B29" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{2B16F7D9-5A0C-174A-9C1B-C57E88FB4BB1}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{448E45C9-02BE-434E-889F-32A10D3374BC}">
+      <formula1>"GenerateOutput, FamilyEntry, IndividualEntry"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{53C292F1-05BE-D749-A667-4F54F4B41106}">
+      <formula1>"GenerateOutputTest"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{ED15F127-3482-FB41-904A-A77BE8F6CCE0}">
+      <formula1>"Coding, Waiting, Completed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -2865,26 +3467,43 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView topLeftCell="C1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>13</v>
@@ -2893,17 +3512,333 @@
         <v>14</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>17</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2">
+        <v>45</v>
+      </c>
+      <c r="F2" s="21">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>46</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+    </row>
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+      <c r="G4">
+        <v>46</v>
+      </c>
+      <c r="H4" s="21">
+        <v>45</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A12" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B23" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B25" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B29" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="B30" s="24" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{3F2C9800-6B5E-014E-B9A1-EA33C975D1B0}">
+      <formula1>"GenerateOutputTest"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{4EA6CE83-FB53-6240-91D7-722AAECF311C}">
+      <formula1>"GenerateOutput, FamilyEntry, IndividualEntry"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{4C89E67B-8BA0-D34F-97CE-82B542713D38}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{6FDC8131-693D-994E-A1B6-DED1DEB4EC61}">
+      <formula1>"Coding, Waiting, Completed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -2911,15 +3846,32 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2944,27 +3896,217 @@
       <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>17</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="F2" s="21"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="18"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+    </row>
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="H4" s="21"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B23" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B25" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B29" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{6ADB0418-EB5B-3549-A05A-90FA10403A88}">
+      <formula1>"GenerateOutputTest"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{6DD15638-6546-3F4F-AC63-4B3A7EFAE151}">
+      <formula1>"GenerateOutput, FamilyEntry, IndividualEntry"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{C80DF632-ECC5-D448-BBB6-9C15686AF69C}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{DDBDEFE7-63CD-434B-AB20-16EAA75B6A41}">
+      <formula1>"Coding, Waiting, Completed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A2" sqref="A2:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2989,504 +4131,694 @@
       <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>17</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="F2" s="21"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="18"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+    </row>
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="H4" s="21"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B23" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B25" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B29" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{18DAA8D5-84BA-0E40-A6A5-3E96345CD927}">
+      <formula1>"GenerateOutputTest"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{7A0F1FD4-299F-6B45-81B5-5D8AFC6651AD}">
+      <formula1>"GenerateOutput, FamilyEntry, IndividualEntry"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{7047A2E0-6B9F-2E4F-A440-7A310039A045}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{92044232-4C77-394F-86A0-C613DE36479E}">
+      <formula1>"Coding, Waiting, Completed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A3" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B5" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="C6" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>113</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="C8" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="12" t="s">
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="12" t="s">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="12" t="s">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="12" t="s">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="12" t="s">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C20" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" t="s">
-        <v>176</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>131</v>
-      </c>
-      <c r="B21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>132</v>
-      </c>
-      <c r="B22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>133</v>
-      </c>
-      <c r="B23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>134</v>
-      </c>
-      <c r="B24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C24" s="12" t="s">
+    </row>
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>135</v>
-      </c>
-      <c r="B25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C25" s="12" t="s">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>136</v>
-      </c>
-      <c r="B26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" s="12" t="s">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>137</v>
-      </c>
-      <c r="B27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>138</v>
-      </c>
-      <c r="B28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" s="12" t="s">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>139</v>
-      </c>
-      <c r="B29" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
         <v>140</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B34" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C34" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
         <v>141</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>142</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C36" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>143</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C37" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>144</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C38" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>145</v>
-      </c>
-      <c r="B35" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="12" t="s">
+      <c r="C39" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
         <v>146</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B40" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
         <v>147</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B41" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C41" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>148</v>
+      </c>
+      <c r="B42" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>148</v>
-      </c>
-      <c r="B38" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38" s="12" t="s">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>149</v>
-      </c>
-      <c r="B39" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>150</v>
-      </c>
-      <c r="B40" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>151</v>
-      </c>
-      <c r="B41" t="s">
-        <v>106</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>152</v>
-      </c>
-      <c r="B42" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>153</v>
-      </c>
-      <c r="B43" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{CBA4C0C8-C552-1747-8B56-4E1F2C52738C}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>